<commit_message>
Update FF_ProFlex_Resource_Planning - 100% eFreight.xlsx
</commit_message>
<xml_diff>
--- a/FF_ProFlex_Resource_Planning - 100% eFreight.xlsx
+++ b/FF_ProFlex_Resource_Planning - 100% eFreight.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U537227\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U537227\Work Folders\Documents\GitHub\GitXLTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2220,7 +2220,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC31" sqref="AC31"/>
+      <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.600000000000001" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -5839,11 +5839,11 @@
       </c>
       <c r="G32" s="29">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="H32" s="29">
         <f t="shared" si="4"/>
-        <v>0.75068493150684934</v>
+        <v>0.87579908675799101</v>
       </c>
       <c r="I32" s="28">
         <f t="array" ref="I32">IF(SUM($L32:$AO32)=0,"",INDEX($L$2:$AO$2,MATCH(FALSE,ISBLANK($L32:$AO32),0)))</f>
@@ -5861,7 +5861,7 @@
         <v>0.5</v>
       </c>
       <c r="M32" s="27">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="N32" s="27">
         <v>0.5</v>
@@ -64711,21 +64711,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100878EF1C29AB0A24AB587BC1DFEEB65B5" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd6ead137c42c2015227dd302e1775ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ebea240f-dd28-4b0e-9da6-71444763d833" xmlns:ns3="e011f290-5bbc-400f-9a77-13cc1174eacf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7610d63ffb3d6602c898b2a0e45ab3c7" ns2:_="" ns3:_="">
     <xsd:import namespace="ebea240f-dd28-4b0e-9da6-71444763d833"/>
@@ -64942,10 +64927,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E947359B-3257-4DD4-808B-BE9378ADEEAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BE1E0C1-3EC2-4ED1-B2F2-E592ABAA0629}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ebea240f-dd28-4b0e-9da6-71444763d833"/>
+    <ds:schemaRef ds:uri="e011f290-5bbc-400f-9a77-13cc1174eacf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -64968,20 +64979,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0BE1E0C1-3EC2-4ED1-B2F2-E592ABAA0629}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E947359B-3257-4DD4-808B-BE9378ADEEAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ebea240f-dd28-4b0e-9da6-71444763d833"/>
-    <ds:schemaRef ds:uri="e011f290-5bbc-400f-9a77-13cc1174eacf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>